<commit_message>
Actualización de metricas de kanban
</commit_message>
<xml_diff>
--- a/Documentacion/kanban-metrics.xlsx
+++ b/Documentacion/kanban-metrics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Column counts</t>
   </si>
@@ -151,6 +151,27 @@
   </si>
   <si>
     <t>HU9</t>
+  </si>
+  <si>
+    <t>HU10</t>
+  </si>
+  <si>
+    <t>HU6</t>
+  </si>
+  <si>
+    <t>HU13</t>
+  </si>
+  <si>
+    <t>HU14</t>
+  </si>
+  <si>
+    <t>HU19</t>
+  </si>
+  <si>
+    <t>HU20</t>
+  </si>
+  <si>
+    <t>HU21</t>
   </si>
 </sst>
 </file>
@@ -502,7 +523,7 @@
                   <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -822,11 +843,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2097206264"/>
-        <c:axId val="2097203080"/>
+        <c:axId val="2097234920"/>
+        <c:axId val="2109701992"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2097206264"/>
+        <c:axId val="2097234920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -836,7 +857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097203080"/>
+        <c:crossAx val="2109701992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -844,7 +865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097203080"/>
+        <c:axId val="2109701992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097206264"/>
+        <c:crossAx val="2097234920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1010,11 +1031,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100009000"/>
-        <c:axId val="2100011944"/>
+        <c:axId val="2097217368"/>
+        <c:axId val="2109204328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2100009000"/>
+        <c:axId val="2097217368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1023,7 +1044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100011944"/>
+        <c:crossAx val="2109204328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1031,7 +1052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100011944"/>
+        <c:axId val="2109204328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,7 +1063,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100009000"/>
+        <c:crossAx val="2097217368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1114,7 +1135,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$41:$B$50</c:f>
+              <c:f>Sheet1!$B$48:$B$57</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1152,7 +1173,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$41:$C$50</c:f>
+              <c:f>Sheet1!$C$48:$C$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1199,8 +1220,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="2100042136"/>
-        <c:axId val="2100045192"/>
+        <c:axId val="2097217848"/>
+        <c:axId val="2097302456"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1210,7 +1231,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$40</c:f>
+              <c:f>Sheet1!$E$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1224,7 +1245,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$41:$E$50</c:f>
+              <c:f>Sheet1!$E$48:$E$57</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1273,11 +1294,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100051528"/>
-        <c:axId val="2100048168"/>
+        <c:axId val="2108811368"/>
+        <c:axId val="2109668456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2100042136"/>
+        <c:axId val="2097217848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,7 +1308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100045192"/>
+        <c:crossAx val="2097302456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1295,7 +1316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100045192"/>
+        <c:axId val="2097302456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,13 +1327,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100042136"/>
+        <c:crossAx val="2097217848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2100048168"/>
+        <c:axId val="2109668456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1323,12 +1344,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100051528"/>
+        <c:crossAx val="2108811368"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2100051528"/>
+        <c:axId val="2108811368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100048168"/>
+        <c:crossAx val="2109668456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1585,11 +1606,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2100077896"/>
-        <c:axId val="2100080872"/>
+        <c:axId val="2097237944"/>
+        <c:axId val="2109119864"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2100077896"/>
+        <c:axId val="2097237944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1599,7 +1620,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100080872"/>
+        <c:crossAx val="2109119864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1607,7 +1628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100080872"/>
+        <c:axId val="2109119864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1618,7 +1639,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100077896"/>
+        <c:crossAx val="2097237944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1706,13 +1727,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>82590</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>93496</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>70123</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>93497</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2089,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T54"/>
+  <dimension ref="B2:T61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="94" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2332,10 +2353,18 @@
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7</v>
+      </c>
       <c r="N9" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2371,7 +2400,7 @@
       </c>
       <c r="O10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P10" s="3">
         <f t="shared" si="2"/>
@@ -2557,7 +2586,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" ref="E18:E37" si="5">D18-C18</f>
+        <f t="shared" ref="E18:E44" si="5">D18-C18</f>
         <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -2907,231 +2936,357 @@
       </c>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="2:12" ht="18">
-      <c r="B39" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="H39" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
+      <c r="B38" s="3">
+        <v>22</v>
+      </c>
+      <c r="C38" s="3">
+        <v>9</v>
+      </c>
+      <c r="D38" s="3">
+        <v>10</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="B39" s="3">
+        <v>23</v>
+      </c>
+      <c r="C39" s="3">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3">
+        <v>10</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="B40" s="3">
+        <v>24</v>
+      </c>
+      <c r="C40" s="3">
         <v>10</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="3">
         <v>10</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="2:12">
       <c r="B41" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C41" s="3">
-        <f>COUNTIF(E$17:E$26,"="&amp;B41)</f>
-        <v>4</v>
-      </c>
-      <c r="D41" s="5">
-        <f>C41</f>
-        <v>4</v>
-      </c>
-      <c r="E41" s="6">
-        <f>D41/D$50</f>
-        <v>0.8</v>
+        <v>10</v>
+      </c>
+      <c r="D41" s="3">
+        <v>10</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="2:12">
       <c r="B42" s="3">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" ref="C42:C49" si="6">COUNTIF(E$17:E$26,"="&amp;B42)</f>
-        <v>1</v>
-      </c>
-      <c r="D42" s="5">
-        <f>D41+C42</f>
-        <v>5</v>
-      </c>
-      <c r="E42" s="6">
-        <f t="shared" ref="E42:E50" si="7">D42/D$50</f>
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D42" s="3">
+        <v>10</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="2:12">
       <c r="B43" s="3">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D43" s="5">
-        <f t="shared" ref="D43:D50" si="8">D42+C43</f>
-        <v>5</v>
-      </c>
-      <c r="E43" s="6">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D43" s="3">
+        <v>10</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="2:12">
       <c r="B44" s="3">
+        <v>28</v>
+      </c>
+      <c r="C44" s="3">
+        <v>10</v>
+      </c>
+      <c r="D44" s="3">
+        <v>10</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="2:12" ht="18">
+      <c r="B46" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="H46" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="B47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3">
+        <f>COUNTIF(E$17:E$26,"="&amp;B48)</f>
         <v>4</v>
       </c>
-      <c r="C44" s="3">
+      <c r="D48" s="5">
+        <f>C48</f>
+        <v>4</v>
+      </c>
+      <c r="E48" s="6">
+        <f>D48/D$57</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" s="3">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" ref="C49:C56" si="6">COUNTIF(E$17:E$26,"="&amp;B49)</f>
+        <v>1</v>
+      </c>
+      <c r="D49" s="5">
+        <f>D48+C49</f>
+        <v>5</v>
+      </c>
+      <c r="E49" s="6">
+        <f t="shared" ref="E49:E57" si="7">D49/D$57</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" s="3">
+        <v>3</v>
+      </c>
+      <c r="C50" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D50" s="5">
+        <f t="shared" ref="D50:D57" si="8">D49+C50</f>
+        <v>5</v>
+      </c>
+      <c r="E50" s="6">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" s="3">
+        <v>4</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="5">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E51" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:12">
-      <c r="B45" s="3">
+    <row r="52" spans="2:5">
+      <c r="B52" s="3">
         <v>5</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C52" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D52" s="5">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E52" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:12">
-      <c r="B46" s="3">
+    <row r="53" spans="2:5">
+      <c r="B53" s="3">
         <v>6</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C53" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D53" s="5">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E53" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:12">
-      <c r="B47" s="3">
+    <row r="54" spans="2:5">
+      <c r="B54" s="3">
         <v>7</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C54" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D54" s="5">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E54" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:12">
-      <c r="B48" s="3">
+    <row r="55" spans="2:5">
+      <c r="B55" s="3">
         <v>8</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C55" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D55" s="5">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E55" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="3">
+    <row r="56" spans="2:5">
+      <c r="B56" s="3">
         <v>9</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C56" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D56" s="5">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E56" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="3" t="s">
+    <row r="57" spans="2:5">
+      <c r="B57" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C57" s="3">
         <f>COUNTIF(E$17:E$26,"&gt;=10")</f>
         <v>0</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D57" s="5">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E57" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="1" t="s">
+    <row r="59" spans="2:5">
+      <c r="B59" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D59" s="1">
         <f>AVERAGE(E17:E26)</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
-      <c r="B53" s="1" t="s">
+    <row r="60" spans="2:5">
+      <c r="B60" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D53" s="4">
-        <f>2/D52</f>
+      <c r="D60" s="4">
+        <f>2/D59</f>
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="54" spans="2:5">
-      <c r="B54" s="1" t="s">
+    <row r="61" spans="2:5">
+      <c r="B61" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D61" s="1">
         <f>PERCENTILE(E17:E26, 0.85)</f>
         <v>1</v>
       </c>
@@ -3142,8 +3297,8 @@
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="H15:L15"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="H46:L46"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>